<commit_message>
remove the achieve system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelInfo.xlsx
+++ b/ConfigData/Xlsx/LevelInfo.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="LevelInfo" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>|您可以|Red|编辑你的卡片||了，选择你喜欢的卡片痛痛快快的战斗吧！</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>|您可以进行|Blue|游戏问答||了。通过游戏问答中回答问题，您可以获得一定的|Cyan|阅历||。</t>
-  </si>
-  <si>
-    <t>|您可以查看您的|Gold|成就||了。只要完成各个成就，您便可以获得|Cyan|钻石||作为奖励！</t>
   </si>
   <si>
     <t>int</t>
@@ -92,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1020,17 +1017,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:E11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A3:E11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:E12">
-    <sortCondition ref="A3:A12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A3:E10"/>
+  <sortState ref="A4:E11">
+    <sortCondition ref="A3:A11"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Level" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Des" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Icon" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="4"/>
+    <tableColumn id="2" name="Level" dataDxfId="3"/>
+    <tableColumn id="3" name="Type" dataDxfId="2"/>
+    <tableColumn id="4" name="Des" dataDxfId="1"/>
+    <tableColumn id="5" name="Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1356,11 +1353,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1373,53 +1370,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -1467,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="7">
         <v>3</v>
@@ -1526,35 +1523,18 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E10" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7">
-        <v>50</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="7">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optimise the level infos
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelInfo.xlsx
+++ b/ConfigData/Xlsx/LevelInfo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>|您可以|Red|编辑你的卡片||了，选择你喜欢的卡片痛痛快快的战斗吧！</t>
   </si>
@@ -92,13 +92,52 @@
   <si>
     <t>|新职业-|Gold|Job||，已经可以使用。可以通过城堡面板，转职按钮来完成|Red|转职||。</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|您可以通过城堡面板，加强自己的防御力量。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>deck</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fight</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cshop</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ques</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cardb</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>job</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>castle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +321,13 @@
       <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -754,7 +800,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -783,6 +829,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1036,10 +1085,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A3:E12"/>
-  <sortState ref="A4:E11">
-    <sortCondition ref="A3:A11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A3:E13"/>
+  <sortState ref="A4:E12">
+    <sortCondition ref="A3:A12"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="Id" dataDxfId="4"/>
@@ -1373,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1451,81 +1500,81 @@
       <c r="D4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="7">
-        <v>1</v>
+      <c r="E4" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="7">
+      <c r="A5" s="10">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="10">
         <v>3</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="10">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="9">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="9">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
+      <c r="A7" s="10">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
-        <v>10</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="C7" s="9">
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="7">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="7">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="7">
-        <v>7</v>
+      <c r="A9" s="10">
+        <v>6</v>
       </c>
       <c r="B9" s="7">
         <v>20</v>
@@ -1534,49 +1583,49 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="7">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="7">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="7">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="B11" s="7">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C11" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="7">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="7">
         <v>0</v>
@@ -1585,17 +1634,35 @@
         <v>2</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="7">
+        <v>101</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="7">
-        <v>11</v>
+      <c r="E13" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove the spinbox from events
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/LevelInfo.xlsx
+++ b/ConfigData/Xlsx/LevelInfo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F4EFB50A-4432-4B83-9902-C7B9E60E48DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LevelInfo" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>|您可以|Red|编辑你的卡片||了，选择你喜欢的卡片痛痛快快的战斗吧！</t>
   </si>
@@ -131,12 +132,16 @@
   </si>
   <si>
     <t>castle</t>
+  </si>
+  <si>
+    <t>|您可以通过幸运转盘面板，获取更多资源和道具。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -328,6 +333,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1085,17 +1091,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A3:E13"/>
-  <sortState ref="A4:E12">
-    <sortCondition ref="A3:A12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:E14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A3:E14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A4:E13">
+    <sortCondition ref="A3:A13"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Id" dataDxfId="4"/>
-    <tableColumn id="2" name="Level" dataDxfId="3"/>
-    <tableColumn id="3" name="Type" dataDxfId="2"/>
-    <tableColumn id="4" name="Des" dataDxfId="1"/>
-    <tableColumn id="5" name="Icon" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Level" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Des" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1421,11 +1427,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1559,38 +1565,38 @@
       <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="7">
-        <v>10</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B8" s="9">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9">
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="10">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
       <c r="B9" s="7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
+      <c r="A10" s="10">
         <v>7</v>
       </c>
       <c r="B10" s="7">
@@ -1600,10 +1606,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -1611,38 +1617,38 @@
         <v>8</v>
       </c>
       <c r="B11" s="7">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7">
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="B12" s="7">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="7">
         <v>0</v>
@@ -1651,9 +1657,26 @@
         <v>2</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="7">
+        <v>101</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>